<commit_message>
Updated Components growth and just adjusted the starting price for scallops in the app
</commit_message>
<xml_diff>
--- a/Components_V4.xlsx
+++ b/Components_V4.xlsx
@@ -20,7 +20,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId16" roundtripDataChecksum="EGqrxQQvnk3r20YKcxWGTgmue3uox4y3DZ+5E5C8BjI="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId16" roundtripDataChecksum="y/S1SnPXTNcg9eMjx5/3dSRbRYu806YnBWOs6eotOsg="/>
     </ext>
   </extLst>
 </workbook>
@@ -43,7 +43,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhoob5v/lO2KgUeISmWyzqmIb7W7g=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mh4u1lH1ikHTQ/qWrb6yO9DHdSeLw=="/>
     </ext>
   </extLst>
 </comments>
@@ -66,7 +66,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhi3qBdWk7Lrm7KLSTNEaYdq6HSBA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhxVwVztZf2HTIud/WqJNXXipKb7w=="/>
     </ext>
   </extLst>
 </comments>
@@ -1554,7 +1554,6 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -1911,7 +1910,6 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.43"/>
     <col customWidth="1" min="2" max="2" width="26.14"/>
     <col customWidth="1" min="3" max="4" width="9.29"/>
     <col customWidth="1" min="5" max="5" width="25.0"/>
@@ -3510,7 +3508,6 @@
     <col customWidth="1" min="1" max="1" width="21.0"/>
     <col customWidth="1" min="2" max="2" width="7.0"/>
     <col customWidth="1" min="3" max="3" width="20.57"/>
-    <col customWidth="1" min="4" max="6" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4778,9 +4775,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="3" width="14.43"/>
     <col customWidth="1" min="4" max="4" width="49.57"/>
-    <col customWidth="1" min="5" max="6" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -7571,11 +7566,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.43"/>
     <col customWidth="1" min="2" max="2" width="26.0"/>
     <col customWidth="1" min="3" max="3" width="11.57"/>
     <col customWidth="1" min="4" max="4" width="12.71"/>
-    <col customWidth="1" min="5" max="5" width="14.43"/>
     <col customWidth="1" min="6" max="6" width="42.43"/>
     <col customWidth="1" min="7" max="7" width="9.29"/>
     <col customWidth="1" min="8" max="8" width="8.71"/>
@@ -11322,10 +11315,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="22.71"/>
-    <col customWidth="1" min="2" max="2" width="14.43"/>
     <col customWidth="1" min="3" max="3" width="21.43"/>
     <col customWidth="1" min="4" max="4" width="22.71"/>
-    <col customWidth="1" min="5" max="6" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -14772,11 +14763,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="32.29"/>
-    <col customWidth="1" min="2" max="2" width="14.43"/>
     <col customWidth="1" min="3" max="3" width="20.29"/>
-    <col customWidth="1" min="4" max="4" width="14.43"/>
     <col customWidth="1" min="5" max="5" width="30.29"/>
-    <col customWidth="1" min="6" max="6" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -17636,9 +17624,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="14.43"/>
     <col customWidth="1" min="3" max="4" width="21.43"/>
-    <col customWidth="1" min="5" max="6" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>